<commit_message>
feat: insert dicts functional
</commit_message>
<xml_diff>
--- a/app/database/insert_dicts/data/violations_dict.xlsx
+++ b/app/database/insert_dicts/data/violations_dict.xlsx
@@ -927,7 +927,7 @@
       </c>
       <c r="J10" s="2" t="inlineStr">
         <is>
-          <t>7 дней</t>
+          <t>7 days</t>
         </is>
       </c>
     </row>
@@ -1011,7 +1011,7 @@
       </c>
       <c r="J12" s="2" t="inlineStr">
         <is>
-          <t>7 дней</t>
+          <t>7 days</t>
         </is>
       </c>
     </row>
@@ -1263,7 +1263,7 @@
       </c>
       <c r="J18" s="2" t="inlineStr">
         <is>
-          <t>7 дней</t>
+          <t>7 days</t>
         </is>
       </c>
     </row>
@@ -1515,7 +1515,7 @@
       </c>
       <c r="J24" s="2" t="inlineStr">
         <is>
-          <t>7 дней</t>
+          <t>7 days</t>
         </is>
       </c>
     </row>
@@ -1809,7 +1809,7 @@
       </c>
       <c r="J31" s="2" t="inlineStr">
         <is>
-          <t>7 дней</t>
+          <t>7 days</t>
         </is>
       </c>
     </row>
@@ -2355,7 +2355,7 @@
       </c>
       <c r="J44" s="2" t="inlineStr">
         <is>
-          <t>7 дней</t>
+          <t>7 days</t>
         </is>
       </c>
     </row>
@@ -2439,7 +2439,7 @@
       </c>
       <c r="J46" s="2" t="inlineStr">
         <is>
-          <t>7 дней</t>
+          <t>7 days</t>
         </is>
       </c>
     </row>
@@ -2691,7 +2691,7 @@
       </c>
       <c r="J52" s="2" t="inlineStr">
         <is>
-          <t>7 дней</t>
+          <t>7 days</t>
         </is>
       </c>
     </row>
@@ -2775,7 +2775,7 @@
       </c>
       <c r="J54" s="2" t="inlineStr">
         <is>
-          <t>7 дней</t>
+          <t>7 days</t>
         </is>
       </c>
     </row>
@@ -2859,7 +2859,7 @@
       </c>
       <c r="J56" s="2" t="inlineStr">
         <is>
-          <t>7 дней</t>
+          <t>7 days</t>
         </is>
       </c>
     </row>
@@ -3111,7 +3111,7 @@
       </c>
       <c r="J62" s="2" t="inlineStr">
         <is>
-          <t>7 дней</t>
+          <t>7 days</t>
         </is>
       </c>
     </row>
@@ -3151,7 +3151,11 @@
       <c r="I63" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J63" s="2" t="inlineStr"/>
+      <c r="J63" s="2" t="inlineStr">
+        <is>
+          <t>5 minutes</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="inlineStr">
@@ -3231,7 +3235,11 @@
       <c r="I65" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J65" s="2" t="inlineStr"/>
+      <c r="J65" s="2" t="inlineStr">
+        <is>
+          <t>5 minutes</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="inlineStr">
@@ -3439,7 +3447,7 @@
       </c>
       <c r="J70" s="2" t="inlineStr">
         <is>
-          <t>7 дней</t>
+          <t>7 days</t>
         </is>
       </c>
     </row>
@@ -3691,7 +3699,7 @@
       </c>
       <c r="J76" s="2" t="inlineStr">
         <is>
-          <t>7 дней</t>
+          <t>7 days</t>
         </is>
       </c>
     </row>
@@ -4069,7 +4077,7 @@
       </c>
       <c r="J85" s="2" t="inlineStr">
         <is>
-          <t>7 дней</t>
+          <t>7 days</t>
         </is>
       </c>
     </row>
@@ -4153,7 +4161,7 @@
       </c>
       <c r="J87" s="2" t="inlineStr">
         <is>
-          <t>7 дней</t>
+          <t>7 days</t>
         </is>
       </c>
     </row>
@@ -4321,7 +4329,7 @@
       </c>
       <c r="J91" s="2" t="inlineStr">
         <is>
-          <t>7 дней</t>
+          <t>7 days</t>
         </is>
       </c>
     </row>
@@ -4489,7 +4497,7 @@
       </c>
       <c r="J95" s="2" t="inlineStr">
         <is>
-          <t>7 дней</t>
+          <t>7 days</t>
         </is>
       </c>
     </row>
@@ -4657,7 +4665,7 @@
       </c>
       <c r="J99" s="2" t="inlineStr">
         <is>
-          <t>7 дней</t>
+          <t>7 days</t>
         </is>
       </c>
     </row>
@@ -4825,7 +4833,7 @@
       </c>
       <c r="J103" s="2" t="inlineStr">
         <is>
-          <t>7 дней</t>
+          <t>7 days</t>
         </is>
       </c>
     </row>
@@ -4909,7 +4917,7 @@
       </c>
       <c r="J105" s="2" t="inlineStr">
         <is>
-          <t>7 дней</t>
+          <t>7 days</t>
         </is>
       </c>
     </row>
@@ -4993,7 +5001,7 @@
       </c>
       <c r="J107" s="2" t="inlineStr">
         <is>
-          <t>7 дней</t>
+          <t>7 days</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: vilation dict changes
</commit_message>
<xml_diff>
--- a/app/database/insert_dicts/data/violations_dict.xlsx
+++ b/app/database/insert_dicts/data/violations_dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27816"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27820"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\timosii\my_administrator\app\database\insert_dicts\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C3D71D-462A-4168-B0D0-5F33552EB6AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDFA4CCA-9C9C-48E6-A415-EF4FC1BC69CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="812" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" tabRatio="812" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="new" sheetId="1" r:id="rId1"/>
@@ -348,9 +348,6 @@
     <t>Присутствуют видимые течи из систем водоснабжения и водоотведения</t>
   </si>
   <si>
-    <t>Лифтгрязные (при наличии)</t>
-  </si>
-  <si>
     <t>Лифт в неисправном состоянии (при наличии)</t>
   </si>
   <si>
@@ -634,6 +631,9 @@
   </si>
   <si>
     <t>violation_dict_id</t>
+  </si>
+  <si>
+    <t>Лифт грязный (при наличии)</t>
   </si>
 </sst>
 </file>
@@ -1048,8 +1048,8 @@
   <dimension ref="A1:K111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,7 +1064,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1111,7 +1111,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>38</v>
@@ -1146,7 +1146,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>38</v>
@@ -1181,7 +1181,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>38</v>
@@ -1216,7 +1216,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>39</v>
@@ -1251,7 +1251,7 @@
         <v>11</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>38</v>
@@ -1286,7 +1286,7 @@
         <v>13</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>38</v>
@@ -1312,7 +1312,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>10</v>
@@ -1321,7 +1321,7 @@
         <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>38</v>
@@ -1382,7 +1382,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>10</v>
@@ -1391,7 +1391,7 @@
         <v>16</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>38</v>
@@ -1417,7 +1417,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>10</v>
@@ -1426,7 +1426,7 @@
         <v>11</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>38</v>
@@ -1461,7 +1461,7 @@
         <v>18</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>38</v>
@@ -1496,7 +1496,7 @@
         <v>18</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>38</v>
@@ -1531,7 +1531,7 @@
         <v>18</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>38</v>
@@ -1566,7 +1566,7 @@
         <v>11</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>38</v>
@@ -1601,7 +1601,7 @@
         <v>13</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>39</v>
@@ -1636,7 +1636,7 @@
         <v>11</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>38</v>
@@ -1671,7 +1671,7 @@
         <v>18</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>38</v>
@@ -1697,7 +1697,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>20</v>
@@ -1706,7 +1706,7 @@
         <v>14</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>38</v>
@@ -1776,7 +1776,7 @@
         <v>13</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>38</v>
@@ -1811,7 +1811,7 @@
         <v>23</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>39</v>
@@ -1872,7 +1872,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>20</v>
@@ -1881,7 +1881,7 @@
         <v>16</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>38</v>
@@ -1916,7 +1916,7 @@
         <v>24</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>39</v>
@@ -1951,7 +1951,7 @@
         <v>11</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>38</v>
@@ -1986,7 +1986,7 @@
         <v>13</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>39</v>
@@ -2021,7 +2021,7 @@
         <v>11</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>38</v>
@@ -2056,7 +2056,7 @@
         <v>11</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>38</v>
@@ -2082,7 +2082,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>20</v>
@@ -2091,7 +2091,7 @@
         <v>11</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>38</v>
@@ -2126,7 +2126,7 @@
         <v>18</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>38</v>
@@ -2161,7 +2161,7 @@
         <v>18</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>38</v>
@@ -2196,7 +2196,7 @@
         <v>18</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>38</v>
@@ -2231,7 +2231,7 @@
         <v>11</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>38</v>
@@ -2266,7 +2266,7 @@
         <v>11</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>38</v>
@@ -2301,7 +2301,7 @@
         <v>24</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>39</v>
@@ -2336,7 +2336,7 @@
         <v>11</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>38</v>
@@ -2371,7 +2371,7 @@
         <v>11</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>38</v>
@@ -2406,7 +2406,7 @@
         <v>11</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>38</v>
@@ -2441,7 +2441,7 @@
         <v>11</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>38</v>
@@ -2476,7 +2476,7 @@
         <v>13</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>39</v>
@@ -2511,7 +2511,7 @@
         <v>13</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>39</v>
@@ -2546,7 +2546,7 @@
         <v>18</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>38</v>
@@ -2581,7 +2581,7 @@
         <v>18</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>38</v>
@@ -2616,7 +2616,7 @@
         <v>11</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>38</v>
@@ -2651,7 +2651,7 @@
         <v>18</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>38</v>
@@ -2721,7 +2721,7 @@
         <v>13</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>38</v>
@@ -2756,7 +2756,7 @@
         <v>23</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>39</v>
@@ -2791,7 +2791,7 @@
         <v>11</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>38</v>
@@ -2826,7 +2826,7 @@
         <v>13</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>38</v>
@@ -2852,7 +2852,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>27</v>
@@ -2861,7 +2861,7 @@
         <v>16</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>38</v>
@@ -2896,7 +2896,7 @@
         <v>11</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>38</v>
@@ -2931,7 +2931,7 @@
         <v>13</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>39</v>
@@ -2957,7 +2957,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>27</v>
@@ -2966,7 +2966,7 @@
         <v>11</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>38</v>
@@ -3001,7 +3001,7 @@
         <v>18</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>38</v>
@@ -3036,7 +3036,7 @@
         <v>18</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>38</v>
@@ -3071,7 +3071,7 @@
         <v>18</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>38</v>
@@ -3106,7 +3106,7 @@
         <v>11</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>38</v>
@@ -3141,7 +3141,7 @@
         <v>11</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>38</v>
@@ -3167,7 +3167,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>29</v>
@@ -3176,7 +3176,7 @@
         <v>18</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>38</v>
@@ -3211,7 +3211,7 @@
         <v>16</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>39</v>
@@ -3246,7 +3246,7 @@
         <v>23</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>39</v>
@@ -3281,7 +3281,7 @@
         <v>18</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>38</v>
@@ -3316,7 +3316,7 @@
         <v>23</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>39</v>
@@ -3351,7 +3351,7 @@
         <v>11</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>38</v>
@@ -3386,7 +3386,7 @@
         <v>13</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>38</v>
@@ -3412,7 +3412,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>29</v>
@@ -3421,7 +3421,7 @@
         <v>11</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>38</v>
@@ -3447,7 +3447,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>29</v>
@@ -3456,7 +3456,7 @@
         <v>11</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>38</v>
@@ -3491,7 +3491,7 @@
         <v>11</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>38</v>
@@ -3526,7 +3526,7 @@
         <v>18</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>38</v>
@@ -3561,7 +3561,7 @@
         <v>18</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>38</v>
@@ -3596,7 +3596,7 @@
         <v>11</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>38</v>
@@ -3631,7 +3631,7 @@
         <v>11</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>38</v>
@@ -3666,7 +3666,7 @@
         <v>11</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>38</v>
@@ -3701,7 +3701,7 @@
         <v>18</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>38</v>
@@ -3736,7 +3736,7 @@
         <v>11</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>38</v>
@@ -3771,7 +3771,7 @@
         <v>18</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>39</v>
@@ -3806,7 +3806,7 @@
         <v>18</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F79" s="2" t="s">
         <v>38</v>
@@ -3841,7 +3841,7 @@
         <v>18</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>38</v>
@@ -3876,7 +3876,7 @@
         <v>18</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>38</v>
@@ -3911,7 +3911,7 @@
         <v>14</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>39</v>
@@ -3946,7 +3946,7 @@
         <v>14</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>39</v>
@@ -3981,7 +3981,7 @@
         <v>11</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>38</v>
@@ -4016,7 +4016,7 @@
         <v>18</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>38</v>
@@ -4051,7 +4051,7 @@
         <v>18</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F86" s="2" t="s">
         <v>39</v>
@@ -4086,7 +4086,7 @@
         <v>18</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>38</v>
@@ -4121,7 +4121,7 @@
         <v>18</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>38</v>
@@ -4156,7 +4156,7 @@
         <v>18</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>38</v>
@@ -4182,7 +4182,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>30</v>
@@ -4191,7 +4191,7 @@
         <v>11</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>38</v>
@@ -4226,7 +4226,7 @@
         <v>18</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F91" s="2" t="s">
         <v>38</v>
@@ -4252,7 +4252,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>31</v>
@@ -4287,7 +4287,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>31</v>
@@ -4296,7 +4296,7 @@
         <v>32</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>38</v>
@@ -4331,7 +4331,7 @@
         <v>32</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>38</v>
@@ -4366,7 +4366,7 @@
         <v>32</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>39</v>
@@ -4401,7 +4401,7 @@
         <v>32</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F96" s="2" t="s">
         <v>38</v>
@@ -4436,7 +4436,7 @@
         <v>11</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>38</v>
@@ -4471,7 +4471,7 @@
         <v>18</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F98" s="2" t="s">
         <v>38</v>
@@ -4506,7 +4506,7 @@
         <v>18</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F99" s="2" t="s">
         <v>39</v>
@@ -4541,7 +4541,7 @@
         <v>18</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F100" s="2" t="s">
         <v>39</v>
@@ -4576,7 +4576,7 @@
         <v>18</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F101" s="2" t="s">
         <v>38</v>
@@ -4602,7 +4602,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>104</v>
+        <v>199</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>34</v>
@@ -4611,7 +4611,7 @@
         <v>11</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F102" s="2" t="s">
         <v>38</v>
@@ -4637,7 +4637,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>34</v>
@@ -4646,7 +4646,7 @@
         <v>13</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F103" s="2" t="s">
         <v>39</v>
@@ -4672,7 +4672,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>34</v>
@@ -4681,7 +4681,7 @@
         <v>11</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F104" s="2" t="s">
         <v>38</v>
@@ -4707,7 +4707,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>34</v>
@@ -4716,7 +4716,7 @@
         <v>13</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F105" s="2" t="s">
         <v>38</v>
@@ -4742,7 +4742,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>34</v>
@@ -4751,7 +4751,7 @@
         <v>11</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F106" s="2" t="s">
         <v>38</v>
@@ -4777,7 +4777,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>34</v>
@@ -4786,7 +4786,7 @@
         <v>13</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F107" s="2" t="s">
         <v>39</v>
@@ -4812,7 +4812,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>35</v>
@@ -4821,7 +4821,7 @@
         <v>11</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F108" s="2" t="s">
         <v>38</v>
@@ -4847,7 +4847,7 @@
         <v>108</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>35</v>
@@ -4856,7 +4856,7 @@
         <v>18</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F109" s="2" t="s">
         <v>39</v>
@@ -4882,7 +4882,7 @@
         <v>109</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>35</v>
@@ -4891,7 +4891,7 @@
         <v>11</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F110" s="2" t="s">
         <v>38</v>
@@ -4917,7 +4917,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>35</v>

</xml_diff>